<commit_message>
ejemplo de los otros 2 documentos.
</commit_message>
<xml_diff>
--- a/TareasDemo/Sprint.0.ASimpleTODOLIST.TRD.xlsx
+++ b/TareasDemo/Sprint.0.ASimpleTODOLIST.TRD.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TRD" sheetId="1" r:id="rId1"/>
+    <sheet name="Diseño" sheetId="2" r:id="rId2"/>
+    <sheet name="Recursos" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Tarea</t>
   </si>
@@ -37,6 +37,81 @@
   </si>
   <si>
     <t>Planear actividades</t>
+  </si>
+  <si>
+    <t>Plataforma:</t>
+  </si>
+  <si>
+    <t>Apache</t>
+  </si>
+  <si>
+    <t>Lenguaje :</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>Tipo de Aplicacion</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Base de Datos:</t>
+  </si>
+  <si>
+    <t>Numero de Servidores</t>
+  </si>
+  <si>
+    <t>Tipo de Hosting</t>
+  </si>
+  <si>
+    <t>Compartido</t>
+  </si>
+  <si>
+    <t>Incluir aqui la suma de horas a desarrollar</t>
+  </si>
+  <si>
+    <t>Costo por hora hombre</t>
+  </si>
+  <si>
+    <t>Incluir cuando debe de ganarse por programar</t>
+  </si>
+  <si>
+    <t>Licencias y paquetes</t>
+  </si>
+  <si>
+    <t>Si compran alguna libreria o paquete</t>
+  </si>
+  <si>
+    <t>Costo de Desarrollo en Horas Hombre</t>
+  </si>
+  <si>
+    <t>Instalacion de producto</t>
+  </si>
+  <si>
+    <t>Costo de Operacion</t>
+  </si>
+  <si>
+    <t>Estimar que tanto tiempo tardan en instalar el producto y como. Te mando un correo, te administro el hosting etc.</t>
+  </si>
+  <si>
+    <t>Cuanto cuesta el shared hosting, incluir precio de dominio, hosting y cualquier otro gasto recurrente.</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Sumar el Primer pago</t>
+  </si>
+  <si>
+    <t>Anticipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resto </t>
   </si>
 </sst>
 </file>
@@ -391,7 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -459,24 +534,144 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios a TRD. Ejemplo y listado de actividades.
</commit_message>
<xml_diff>
--- a/TareasDemo/Sprint.0.ASimpleTODOLIST.TRD.xlsx
+++ b/TareasDemo/Sprint.0.ASimpleTODOLIST.TRD.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TRD" sheetId="1" r:id="rId1"/>
     <sheet name="Diseño" sheetId="2" r:id="rId2"/>
     <sheet name="Recursos" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Tarea</t>
   </si>
@@ -72,21 +72,12 @@
     <t>Compartido</t>
   </si>
   <si>
-    <t>Incluir aqui la suma de horas a desarrollar</t>
-  </si>
-  <si>
     <t>Costo por hora hombre</t>
   </si>
   <si>
-    <t>Incluir cuando debe de ganarse por programar</t>
-  </si>
-  <si>
     <t>Licencias y paquetes</t>
   </si>
   <si>
-    <t>Si compran alguna libreria o paquete</t>
-  </si>
-  <si>
     <t>Costo de Desarrollo en Horas Hombre</t>
   </si>
   <si>
@@ -96,12 +87,6 @@
     <t>Costo de Operacion</t>
   </si>
   <si>
-    <t>Estimar que tanto tiempo tardan en instalar el producto y como. Te mando un correo, te administro el hosting etc.</t>
-  </si>
-  <si>
-    <t>Cuanto cuesta el shared hosting, incluir precio de dominio, hosting y cualquier otro gasto recurrente.</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -112,6 +97,69 @@
   </si>
   <si>
     <t xml:space="preserve">Resto </t>
+  </si>
+  <si>
+    <t>Lista de tareas</t>
+  </si>
+  <si>
+    <t>Crear tarea</t>
+  </si>
+  <si>
+    <t>Actualizar tarea</t>
+  </si>
+  <si>
+    <t>Comentar</t>
+  </si>
+  <si>
+    <t>Borrar</t>
+  </si>
+  <si>
+    <t>Base de datos</t>
+  </si>
+  <si>
+    <t>Tabla Tareas</t>
+  </si>
+  <si>
+    <t>Tabla Comentarios</t>
+  </si>
+  <si>
+    <t>Ltareas - Leer todos los datos de la base de datos</t>
+  </si>
+  <si>
+    <t>genera html de lista de tareas</t>
+  </si>
+  <si>
+    <t>Incluir menus de navegacion.</t>
+  </si>
+  <si>
+    <t>Formulario de Crear tarea (html)</t>
+  </si>
+  <si>
+    <t>Guardar la tarea en base de datos</t>
+  </si>
+  <si>
+    <t>Formulario de actualizar tarea (Html)</t>
+  </si>
+  <si>
+    <t>Actualizar la tarea en db.</t>
+  </si>
+  <si>
+    <t>Formulatio borrar tarea (html)</t>
+  </si>
+  <si>
+    <t>Borrar tarea de db.</t>
+  </si>
+  <si>
+    <t>Listar comentarios (html)</t>
+  </si>
+  <si>
+    <t>formulario de Comentarios</t>
+  </si>
+  <si>
+    <t>Agregar comentario en DB.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diseñar interface (CSS). </t>
   </si>
 </sst>
 </file>
@@ -164,13 +212,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E15" totalsRowShown="0">
-  <autoFilter ref="A1:E15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E25" totalsRowCount="1">
+  <autoFilter ref="A1:E25"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Tarea"/>
     <tableColumn id="2" name="Funcion"/>
     <tableColumn id="3" name="Descripcion"/>
-    <tableColumn id="4" name="Tiempo Estimado"/>
+    <tableColumn id="4" name="Tiempo Estimado" totalsRowFunction="sum"/>
     <tableColumn id="5" name="Tiempo Actual"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -464,17 +512,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.5546875" customWidth="1"/>
     <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" customWidth="1"/>
   </cols>
@@ -512,7 +560,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -522,6 +570,189 @@
       </c>
       <c r="D3">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <f>SUBTOTAL(109,Table1[Tiempo Estimado])</f>
+        <v>11.5</v>
       </c>
     </row>
   </sheetData>
@@ -536,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,72 +834,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="95.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>11.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios a la lista de actividades. Las actividades principales ya estaban desglosadas por este motivo su tiempo se redujo a cero.
</commit_message>
<xml_diff>
--- a/TareasDemo/Sprint.0.ASimpleTODOLIST.TRD.xlsx
+++ b/TareasDemo/Sprint.0.ASimpleTODOLIST.TRD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="TRD" sheetId="1" r:id="rId1"/>
@@ -213,7 +213,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E25" totalsRowCount="1">
-  <autoFilter ref="A1:E25"/>
+  <autoFilter ref="A1:E24"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Tarea"/>
     <tableColumn id="2" name="Funcion"/>
@@ -514,15 +514,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.5546875" customWidth="1"/>
     <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" customWidth="1"/>
   </cols>
@@ -577,59 +575,92 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
       </c>
       <c r="D5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
       <c r="C7" t="s">
         <v>30</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
       <c r="C8" t="s">
         <v>31</v>
       </c>
       <c r="D8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
       <c r="C9" t="s">
         <v>32</v>
       </c>
       <c r="D9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
       <c r="C10" t="s">
         <v>33</v>
       </c>
@@ -638,6 +669,12 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
       <c r="C11" t="s">
         <v>34</v>
       </c>
@@ -646,6 +683,12 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
       <c r="C12" t="s">
         <v>35</v>
       </c>
@@ -654,6 +697,12 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
       <c r="C13" t="s">
         <v>36</v>
       </c>
@@ -662,6 +711,12 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
       <c r="C14" t="s">
         <v>37</v>
       </c>
@@ -670,6 +725,12 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
       <c r="C15" t="s">
         <v>38</v>
       </c>
@@ -678,6 +739,12 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
       <c r="C16" t="s">
         <v>39</v>
       </c>
@@ -685,7 +752,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
       <c r="C17" t="s">
         <v>40</v>
       </c>
@@ -693,7 +766,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
       <c r="C18" t="s">
         <v>41</v>
       </c>
@@ -701,7 +780,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
       <c r="C19" t="s">
         <v>42</v>
       </c>
@@ -709,7 +794,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
       <c r="C20" t="s">
         <v>43</v>
       </c>
@@ -717,7 +808,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
       <c r="C21" t="s">
         <v>44</v>
       </c>
@@ -725,7 +822,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
       <c r="C22" t="s">
         <v>45</v>
       </c>
@@ -733,7 +836,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
       <c r="C23" t="s">
         <v>46</v>
       </c>
@@ -741,7 +850,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
       <c r="C24" t="s">
         <v>47</v>
       </c>
@@ -749,10 +864,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D25">
         <f>SUBTOTAL(109,Table1[Tiempo Estimado])</f>
-        <v>11.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -768,7 +883,7 @@
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,7 +949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Actualizaciones en la hoja de costos y en arquitectura. se agregaron unos servicios de hosting conocidos.
</commit_message>
<xml_diff>
--- a/TareasDemo/Sprint.0.ASimpleTODOLIST.TRD.xlsx
+++ b/TareasDemo/Sprint.0.ASimpleTODOLIST.TRD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TRD" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Tarea</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Sumar el Primer pago</t>
-  </si>
-  <si>
     <t>Anticipo</t>
   </si>
   <si>
@@ -160,16 +157,60 @@
   </si>
   <si>
     <t xml:space="preserve">Diseñar interface (CSS). </t>
+  </si>
+  <si>
+    <t>Servicios de Hosting :</t>
+  </si>
+  <si>
+    <t>www.godaddy.com</t>
+  </si>
+  <si>
+    <t>www.hostgator.com</t>
+  </si>
+  <si>
+    <t>www.hostdime.com</t>
+  </si>
+  <si>
+    <t>Total desarrollo</t>
+  </si>
+  <si>
+    <t>Godaddy basic mensual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -192,13 +233,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -514,7 +562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -578,7 +626,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -592,7 +640,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -606,7 +654,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -620,7 +668,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -634,7 +682,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -648,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -662,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10">
         <v>0.5</v>
@@ -676,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>0.5</v>
@@ -690,7 +738,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12">
         <v>0.5</v>
@@ -704,7 +752,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13">
         <v>0.5</v>
@@ -718,7 +766,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14">
         <v>0.5</v>
@@ -732,7 +780,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15">
         <v>0.5</v>
@@ -746,7 +794,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <v>0.5</v>
@@ -760,7 +808,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17">
         <v>0.5</v>
@@ -774,7 +822,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18">
         <v>0.5</v>
@@ -788,7 +836,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19">
         <v>0.5</v>
@@ -802,7 +850,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20">
         <v>0.5</v>
@@ -816,7 +864,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21">
         <v>0.5</v>
@@ -830,7 +878,7 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22">
         <v>0.5</v>
@@ -844,7 +892,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23">
         <v>0.5</v>
@@ -858,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24">
         <v>0.5</v>
@@ -880,10 +928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B7"/>
+  <dimension ref="A2:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,17 +988,42 @@
         <v>17</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A14" r:id="rId1"/>
+    <hyperlink ref="A15" r:id="rId2"/>
+    <hyperlink ref="A16" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B13"/>
+  <dimension ref="A3:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,65 +1032,93 @@
     <col min="2" max="2" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B3">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3">
+        <f>B4*B3</f>
+        <v>850</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8">
+      <c r="B9" s="3">
         <v>66</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" s="3">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B13" s="3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>26</v>
+      <c r="B14" s="3">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>